<commit_message>
Mise à jour du dashboard et du code
</commit_message>
<xml_diff>
--- a/Auctions EUA.xlsx
+++ b/Auctions EUA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gvaps1\USR6\CHGE\desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gvaps1\USR6\CHGE\desktop\EUA dashboard 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC19B64E-0328-40C3-9B43-B7BCD40E836C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31D56F1-FC2D-4361-8599-8911FA4FCB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
@@ -905,7 +905,7 @@
         <tr r="I109" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|3943920066704382928|22</stp>
         <stp>UKATOBID Index</stp>
@@ -921,7 +921,7 @@
         <tr r="H101" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|5088816692015618598|22</stp>
         <stp>UKACORAT Index</stp>
@@ -953,7 +953,7 @@
         <tr r="P51" s="2"/>
       </tp>
       <tp>
-        <v>85</v>
+        <v>80</v>
         <stp/>
         <stp>BDP|10519417515402280991|22</stp>
         <stp>EEX3EPPM Index</stp>
@@ -968,6 +968,8 @@
         <stp>BID</stp>
         <tr r="H93" s="2"/>
       </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A Real Time</v>
         <stp/>
@@ -984,6 +986,8 @@
         <stp>ASK</stp>
         <tr r="I101" s="2"/>
       </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
@@ -1057,7 +1061,7 @@
         <tr r="I59" s="2"/>
       </tp>
       <tp>
-        <v>68.05</v>
+        <v>64</v>
         <stp/>
         <stp>BDP|17420742517022627310|22</stp>
         <stp>EEX3X3PL Index</stp>
@@ -1073,7 +1077,7 @@
         <tr r="I113" s="2"/>
       </tp>
       <tp>
-        <v>65</v>
+        <v>73.2</v>
         <stp/>
         <stp>BDP|15420833856443191727|22</stp>
         <stp>EEX3PMDE Index</stp>
@@ -1113,7 +1117,7 @@
         <tr r="P97" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Real Time</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|4461466310551583618|22</stp>
         <stp>RGGIAAQS Index</stp>
@@ -1129,7 +1133,7 @@
         <tr r="H59" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|5161086271000779607|22</stp>
         <stp>EEX3X3PL Index</stp>
@@ -1177,25 +1181,25 @@
         <tr r="H70" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3663603769</v>
+        <v>#N/A Requesting Data...2663367911</v>
         <stp/>
         <stp>BDP|11269571729604204855</stp>
         <tr r="C145" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3405150084</v>
+        <v>#N/A Requesting Data...3647323740</v>
         <stp/>
         <stp>BDP|10943788378258769235</stp>
         <tr r="D109" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1947112609</v>
+        <v>#N/A Requesting Data...4082360482</v>
         <stp/>
         <stp>BDP|13172746922254409863</stp>
         <tr r="O80" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1159917878</v>
+        <v>#N/A Requesting Data...3380412473</v>
         <stp/>
         <stp>BDP|14497910193647682945</stp>
         <tr r="D70" s="2"/>
@@ -1217,7 +1221,7 @@
         <tr r="P69" s="2"/>
       </tp>
       <tp t="s">
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
         <stp/>
         <stp>BDP|3193189600887063507|22</stp>
         <stp>EEX3CRDE Index</stp>
@@ -1225,7 +1229,7 @@
         <tr r="P59" s="2"/>
       </tp>
       <tp>
-        <v>85</v>
+        <v>80</v>
         <stp/>
         <stp>BDP|11258790351540468562|22</stp>
         <stp>EEX3PMEU Index</stp>
@@ -1241,25 +1245,25 @@
         <tr r="H83" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1187855719</v>
+        <v>#N/A Requesting Data...2769441933</v>
         <stp/>
         <stp>BDP|18008250999471656922</stp>
         <tr r="D91" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...765823443</v>
+        <v>#N/A Requesting Data...2816919568</v>
         <stp/>
         <stp>BDP|17732115207434946955</stp>
         <tr r="O35" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1045603430</v>
+        <v>#N/A Requesting Data...3375213175</v>
         <stp/>
         <stp>BDP|17883504586526473761</stp>
         <tr r="D60" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2771171952</v>
+        <v>#N/A Requesting Data...3976777675</v>
         <stp/>
         <stp>BDP|17453411474857561889</stp>
         <tr r="C51" s="2"/>
@@ -1273,25 +1277,25 @@
         <tr r="P123" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3922949328</v>
+        <v>#N/A Requesting Data...3620713657</v>
         <stp/>
         <stp>BDP|17440720740509750509</stp>
         <tr r="D131" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3156595163</v>
+        <v>#N/A Requesting Data...4136725882</v>
         <stp/>
         <stp>BDP|13137573291627110020</stp>
         <tr r="O122" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2725416745</v>
+        <v>#N/A Requesting Data...2448984138</v>
         <stp/>
         <stp>BDP|12589828556680285779</stp>
         <tr r="C131" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4141421577</v>
+        <v>#N/A Requesting Data...3284802481</v>
         <stp/>
         <stp>BDP|14677421799633940220</stp>
         <tr r="D135" s="2"/>
@@ -1313,25 +1317,25 @@
         <tr r="H60" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2918703527</v>
+        <v>#N/A Requesting Data...3867057995</v>
         <stp/>
         <stp>BDP|13392001727258142092</stp>
         <tr r="O125" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3922588643</v>
+        <v>#N/A Requesting Data...2871906050</v>
         <stp/>
         <stp>BDP|14017755899281818256</stp>
         <tr r="D39" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3044361124</v>
+        <v>#N/A Requesting Data...2433242235</v>
         <stp/>
         <stp>BDP|15783964005736454339</stp>
         <tr r="D51" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3053920026</v>
+        <v>#N/A Requesting Data...3424353202</v>
         <stp/>
         <stp>BDP|15365985838177005150</stp>
         <tr r="O49" s="2"/>
@@ -1361,7 +1365,7 @@
         <tr r="I70" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|17032143300330279338|22</stp>
         <stp>UKAAUPR Index</stp>
@@ -1369,19 +1373,19 @@
         <tr r="P35" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2901226881</v>
+        <v>#N/A Requesting Data...2618270724</v>
         <stp/>
         <stp>BDP|15339769723328136685</stp>
         <tr r="C63" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4243433795</v>
+        <v>#N/A Requesting Data...2533842247</v>
         <stp/>
         <stp>BDP|18033101966751297072</stp>
         <tr r="C67" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...555377106</v>
+        <v>#N/A Requesting Data...2509700895</v>
         <stp/>
         <stp>BDP|14450087638141730867</stp>
         <tr r="D59" s="2"/>
@@ -1419,85 +1423,85 @@
         <tr r="I41" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3858241746</v>
+        <v>#N/A Requesting Data...4286009376</v>
         <stp/>
         <stp>BDP|18411307338470386767</stp>
         <tr r="D99" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2624166883</v>
+        <v>#N/A Requesting Data...3489676900</v>
         <stp/>
         <stp>BDP|10666662405090903935</stp>
         <tr r="C107" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2603101695</v>
+        <v>#N/A Requesting Data...2719305007</v>
         <stp/>
         <stp>BDP|14977427384300822780</stp>
         <tr r="O51" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2314933622</v>
+        <v>#N/A Requesting Data...3242892664</v>
         <stp/>
         <stp>BDP|16823031330433881965</stp>
         <tr r="C79" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3891170071</v>
+        <v>#N/A Requesting Data...3675674282</v>
         <stp/>
         <stp>BDP|11920132482670808779</stp>
         <tr r="O121" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1841546203</v>
+        <v>#N/A Requesting Data...3400789991</v>
         <stp/>
         <stp>BDP|16946453695197801084</stp>
         <tr r="D71" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4234647573</v>
+        <v>#N/A Requesting Data...2996594825</v>
         <stp/>
         <stp>BDP|17933236663647161806</stp>
         <tr r="O142" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2741471106</v>
+        <v>#N/A Requesting Data...3157724731</v>
         <stp/>
         <stp>BDP|16760592922515211860</stp>
         <tr r="C135" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...715812412</v>
+        <v>#N/A Requesting Data...2591279903</v>
         <stp/>
         <stp>BDP|17148762016524255989</stp>
         <tr r="C73" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...476282568</v>
+        <v>#N/A Requesting Data...3511501019</v>
         <stp/>
         <stp>BDP|18309468170035994204</stp>
         <tr r="C129" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2357880472</v>
+        <v>#N/A Requesting Data...2759043607</v>
         <stp/>
         <stp>BDP|17271087938758253012</stp>
         <tr r="C57" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1028539393</v>
+        <v>#N/A Requesting Data...2755152195</v>
         <stp/>
         <stp>BDP|12870303344301412882</stp>
         <tr r="C91" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...927394045</v>
+        <v>#N/A Requesting Data...2643477687</v>
         <stp/>
         <stp>BDP|11040138180590694408</stp>
         <tr r="C81" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2570834638</v>
+        <v>#N/A Requesting Data...3171661985</v>
         <stp/>
         <stp>BDP|11220363830214973997</stp>
         <tr r="C50" s="2"/>
@@ -1511,43 +1515,43 @@
         <tr r="I121" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3965657168</v>
+        <v>#N/A Requesting Data...2604302277</v>
         <stp/>
         <stp>BDP|10310929788149374579</stp>
         <tr r="C80" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1650432576</v>
+        <v>#N/A Requesting Data...3998192181</v>
         <stp/>
         <stp>BDP|17645551591513564590</stp>
         <tr r="C119" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2772408717</v>
+        <v>#N/A Requesting Data...3363774490</v>
         <stp/>
         <stp>BDP|11799929507266026330</stp>
         <tr r="C93" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2334827117</v>
+        <v>#N/A Requesting Data...2745243985</v>
         <stp/>
         <stp>BDP|12376569583387116556</stp>
         <tr r="D77" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3852525986</v>
+        <v>#N/A Requesting Data...3165591379</v>
         <stp/>
         <stp>BDP|12929767077087211884</stp>
         <tr r="C90" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4175245610</v>
+        <v>#N/A Requesting Data...2946302355</v>
         <stp/>
         <stp>BDP|12746681013678887006</stp>
         <tr r="C83" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...868216309</v>
+        <v>#N/A Requesting Data...3750072427</v>
         <stp/>
         <stp>BDP|12638693508540193928</stp>
         <tr r="O83" s="2"/>
@@ -1593,19 +1597,19 @@
         <tr r="P133" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...478910447</v>
+        <v>#N/A Requesting Data...3538349847</v>
         <stp/>
         <stp>BDP|17119275309777085060</stp>
         <tr r="D97" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3460763358</v>
+        <v>#N/A Requesting Data...3003669118</v>
         <stp/>
         <stp>BDP|16334400116593439221</stp>
         <tr r="D103" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...694498985</v>
+        <v>#N/A Requesting Data...3222245042</v>
         <stp/>
         <stp>BDP|17261400698320790895</stp>
         <tr r="O123" s="2"/>
@@ -1619,7 +1623,7 @@
         <tr r="P100" s="2"/>
       </tp>
       <tp t="s">
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
         <stp/>
         <stp>BDP|4742737479639692576|22</stp>
         <stp>EEX3BDDE Index</stp>
@@ -1635,49 +1639,49 @@
         <tr r="P128" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1700509852</v>
+        <v>#N/A Requesting Data...3656279741</v>
         <stp/>
         <stp>BDP|10231084159133314599</stp>
         <tr r="O63" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1650628679</v>
+        <v>#N/A Requesting Data...3595582063</v>
         <stp/>
         <stp>BDP|10762113169831043550</stp>
         <tr r="C59" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2761107587</v>
+        <v>#N/A Requesting Data...3710226606</v>
         <stp/>
         <stp>BDP|16233839828067587813</stp>
         <tr r="O69" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...471397057</v>
+        <v>#N/A Requesting Data...4140414659</v>
         <stp/>
         <stp>BDP|18112152192717370493</stp>
         <tr r="D57" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3261907817</v>
+        <v>#N/A Requesting Data...2427535219</v>
         <stp/>
         <stp>BDP|12631048552532555647</stp>
         <tr r="C45" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4120198930</v>
+        <v>#N/A Requesting Data...3555150077</v>
         <stp/>
         <stp>BDP|16257536659004183193</stp>
         <tr r="D61" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2211981438</v>
+        <v>#N/A Requesting Data...4280012389</v>
         <stp/>
         <stp>BDP|11773772447184358568</stp>
         <tr r="D67" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1064173737</v>
+        <v>#N/A Requesting Data...3206967339</v>
         <stp/>
         <stp>BDP|11036023536593262247</stp>
         <tr r="D80" s="2"/>
@@ -1699,7 +1703,7 @@
         <tr r="I69" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1307544468</v>
+        <v>#N/A Requesting Data...3409038685</v>
         <stp/>
         <stp>BDP|10371740171936643690</stp>
         <tr r="C121" s="2"/>
@@ -1729,49 +1733,49 @@
         <tr r="P109" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...603852976</v>
+        <v>#N/A Requesting Data...2848256174</v>
         <stp/>
         <stp>BDP|10450986407190051879</stp>
         <tr r="O113" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1079972701</v>
+        <v>#N/A Requesting Data...4011555900</v>
         <stp/>
         <stp>BDP|17345118041494135735</stp>
         <tr r="O39" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1196633533</v>
+        <v>#N/A Requesting Data...3810880581</v>
         <stp/>
         <stp>BDP|12312559960178218854</stp>
         <tr r="O60" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1049517688</v>
+        <v>#N/A Requesting Data...3049031587</v>
         <stp/>
         <stp>BDP|18235654050928285246</stp>
         <tr r="D118" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...471439640</v>
+        <v>#N/A Requesting Data...3187605494</v>
         <stp/>
         <stp>BDP|11908180946526696355</stp>
         <tr r="O77" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2620354835</v>
+        <v>#N/A Requesting Data...3261991071</v>
         <stp/>
         <stp>BDP|16041498039241224153</stp>
         <tr r="D50" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2857853502</v>
+        <v>#N/A Requesting Data...3297073320</v>
         <stp/>
         <stp>BDP|15600557786638647149</stp>
         <tr r="O135" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1837822420</v>
+        <v>#N/A Requesting Data...4065582076</v>
         <stp/>
         <stp>BDP|17201301560995300668</stp>
         <tr r="C128" s="2"/>
@@ -1801,61 +1805,61 @@
         <tr r="I118" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2101624386</v>
+        <v>#N/A Requesting Data...2799071673</v>
         <stp/>
         <stp>BDP|11964424655954108243</stp>
         <tr r="O152" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3173903063</v>
+        <v>#N/A Requesting Data...4110705262</v>
         <stp/>
         <stp>BDP|15039250998841436929</stp>
         <tr r="C70" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2214083738</v>
+        <v>#N/A Requesting Data...3567892437</v>
         <stp/>
         <stp>BDP|12983476071071398635</stp>
         <tr r="D121" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1085362125</v>
+        <v>#N/A Requesting Data...3866378674</v>
         <stp/>
         <stp>BDP|13022728685482255840</stp>
         <tr r="D151" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2947624395</v>
+        <v>#N/A Requesting Data...3708717750</v>
         <stp/>
         <stp>BDP|14787445835483775602</stp>
         <tr r="C49" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1167837099</v>
+        <v>#N/A Requesting Data...3015514052</v>
         <stp/>
         <stp>BDP|13835889490117150311</stp>
         <tr r="C41" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3905026370</v>
+        <v>#N/A Requesting Data...3375485063</v>
         <stp/>
         <stp>BDP|11777284828983264462</stp>
         <tr r="C152" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4016581608</v>
+        <v>#N/A Requesting Data...3669244062</v>
         <stp/>
         <stp>BDP|16175526658473866307</stp>
         <tr r="O101" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2119254158</v>
+        <v>#N/A Requesting Data...3029214441</v>
         <stp/>
         <stp>BDP|17426017852985395138</stp>
         <tr r="D125" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2677255154</v>
+        <v>#N/A Requesting Data...3766801939</v>
         <stp/>
         <stp>BDP|11679146174687658674</stp>
         <tr r="O61" s="2"/>
@@ -1877,49 +1881,49 @@
         <tr r="I73" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3358321687</v>
+        <v>#N/A Requesting Data...3040314226</v>
         <stp/>
         <stp>BDP|11739412558546315165</stp>
         <tr r="O107" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2643484891</v>
+        <v>#N/A Requesting Data...3558702108</v>
         <stp/>
         <stp>BDP|17821757611616847099</stp>
         <tr r="D73" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1626689338</v>
+        <v>#N/A Requesting Data...2976283069</v>
         <stp/>
         <stp>BDP|12363162891205314891</stp>
         <tr r="C132" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1543122766</v>
+        <v>#N/A Requesting Data...2866850187</v>
         <stp/>
         <stp>BDP|16498489714365827135</stp>
         <tr r="O38" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1701137017</v>
+        <v>#N/A Requesting Data...3726111015</v>
         <stp/>
         <stp>BDP|17756265275154491129</stp>
         <tr r="D152" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2848979254</v>
+        <v>#N/A Requesting Data...3955653838</v>
         <stp/>
         <stp>BDP|11973396237516626030</stp>
         <tr r="D122" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1443475757</v>
+        <v>#N/A Requesting Data...3154516701</v>
         <stp/>
         <stp>BDP|13226662244594317259</stp>
         <tr r="O141" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3191832762</v>
+        <v>#N/A Requesting Data...2971653516</v>
         <stp/>
         <stp>BDP|17779836694136602703</stp>
         <tr r="D69" s="2"/>
@@ -1941,37 +1945,37 @@
         <tr r="H35" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1171746447</v>
+        <v>#N/A Requesting Data...3921764219</v>
         <stp/>
         <stp>BDP|17702743798129095414</stp>
         <tr r="C109" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3306395084</v>
+        <v>#N/A Requesting Data...3122026265</v>
         <stp/>
         <stp>BDP|14502996891943856393</stp>
         <tr r="D107" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...652957546</v>
+        <v>#N/A Requesting Data...3340040318</v>
         <stp/>
         <stp>BDP|14009510159603117373</stp>
         <tr r="C151" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4262266132</v>
+        <v>#N/A Requesting Data...3775661625</v>
         <stp/>
         <stp>BDP|17433439855215748722</stp>
         <tr r="D63" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3578518427</v>
+        <v>#N/A Requesting Data...3880576842</v>
         <stp/>
         <stp>BDP|15963953319790315909</stp>
         <tr r="O132" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1260431136</v>
+        <v>#N/A Requesting Data...3087713912</v>
         <stp/>
         <stp>BDP|10568242787378537653</stp>
         <tr r="O37" s="2"/>
@@ -1985,37 +1989,37 @@
         <tr r="I79" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2959851987</v>
+        <v>#N/A Requesting Data...3151701354</v>
         <stp/>
         <stp>BDP|13291842058863532828</stp>
         <tr r="O70" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...504873358</v>
+        <v>#N/A Requesting Data...4172034269</v>
         <stp/>
         <stp>BDP|12418513149975378324</stp>
         <tr r="C97" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2556372507</v>
+        <v>#N/A Requesting Data...3274033329</v>
         <stp/>
         <stp>BDP|14876410132956204074</stp>
         <tr r="D89" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4180358670</v>
+        <v>#N/A Requesting Data...2803048854</v>
         <stp/>
         <stp>BDP|12662972772298021130</stp>
         <tr r="O41" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3630380519</v>
+        <v>#N/A Requesting Data...3021312028</v>
         <stp/>
         <stp>BDP|15876548244805841436</stp>
         <tr r="O151" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4106067445</v>
+        <v>#N/A Requesting Data...3435174195</v>
         <stp/>
         <stp>BDP|12436206503061465444</stp>
         <tr r="O89" s="2"/>
@@ -2031,7 +2035,7 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Real Time</v>
+        <v>#N/A N/A</v>
         <stp/>
         <stp>BDP|677811009837369073|22</stp>
         <stp>RGGIAAQS Index</stp>
@@ -2039,7 +2043,7 @@
         <tr r="I145" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|14673752842554335912|22</stp>
         <stp>UKASBBID Index</stp>
@@ -2095,7 +2099,7 @@
         <tr r="H81" s="2"/>
       </tp>
       <tp>
-        <v>64</v>
+        <v>68</v>
         <stp/>
         <stp>BDP|8894173801250207596|22</stp>
         <stp>EEX3PMEU Index</stp>
@@ -2135,7 +2139,7 @@
         <tr r="P121" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|1983300863809941800|22</stp>
         <stp>UKABIDS Index</stp>
@@ -2151,7 +2155,7 @@
         <tr r="H132" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|558483427366924145|22</stp>
         <stp>EEX3MNPL Index</stp>
@@ -2159,7 +2163,7 @@
         <tr r="P90" s="2"/>
       </tp>
       <tp t="s">
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
         <stp/>
         <stp>BDP|14840393295774202550|22</stp>
         <stp>EEX3PMDE Index</stp>
@@ -2276,8 +2280,8 @@
         <stp>BDP|13384680936024714500|22</stp>
         <stp>ACCUABAP Index</stp>
         <stp>TIME</stp>
+        <tr r="P28" s="2"/>
         <tr r="P149" s="2"/>
-        <tr r="P28" s="2"/>
       </tp>
       <tp t="s">
         <v>11:00:00</v>
@@ -2320,7 +2324,7 @@
         <tr r="P152" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|15098924859057617101|22</stp>
         <stp>EEX3BDPL Index</stp>
@@ -2336,7 +2340,7 @@
         <tr r="P79" s="2"/>
       </tp>
       <tp t="s">
-        <v>11:00:32</v>
+        <v>11:00:34</v>
         <stp/>
         <stp>BDP|15913837711201520928|22</stp>
         <stp>EEX3EPPM Index</stp>
@@ -2360,7 +2364,7 @@
         <tr r="P132" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|10360780237680756815|22</stp>
         <stp>EEX3MDPL Index</stp>
@@ -2424,7 +2428,7 @@
         <tr r="H110" s="2"/>
       </tp>
       <tp t="s">
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
         <stp/>
         <stp>BDP|12484327023668429337|22</stp>
         <stp>EEX3MNDE Index</stp>
@@ -2448,7 +2452,7 @@
         <tr r="H50" s="2"/>
       </tp>
       <tp>
-        <v>64</v>
+        <v>68</v>
         <stp/>
         <stp>BDP|4673945679228878777|22</stp>
         <stp>EEX3EPPM Index</stp>
@@ -2464,7 +2468,7 @@
         <tr r="P103" s="2"/>
       </tp>
       <tp t="s">
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
         <stp/>
         <stp>BDP|10597827675332248545|22</stp>
         <stp>EEX3MDDE Index</stp>
@@ -2472,49 +2476,49 @@
         <tr r="P61" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...961189930</v>
+        <v>#N/A Requesting Data...3355053286</v>
         <stp/>
         <stp>BDP|4124903069222755554</stp>
         <tr r="O87" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2830793185</v>
+        <v>#N/A Requesting Data...3514438771</v>
         <stp/>
         <stp>BDP|8892146774205393713</stp>
         <tr r="D129" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4092154008</v>
+        <v>#N/A Requesting Data...2989595048</v>
         <stp/>
         <stp>BDP|2477959445181429293</stp>
         <tr r="O129" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1420091099</v>
+        <v>#N/A Requesting Data...4041781125</v>
         <stp/>
         <stp>BDP|9350291445254965784</stp>
         <tr r="D37" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2436070617</v>
+        <v>#N/A Requesting Data...4292275806</v>
         <stp/>
         <stp>BDP|6891918115273664161</stp>
         <tr r="D139" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3559965846</v>
+        <v>#N/A Requesting Data...2689734089</v>
         <stp/>
         <stp>BDP|3573415783287593449</stp>
         <tr r="C48" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4096416158</v>
+        <v>#N/A Requesting Data...2954003455</v>
         <stp/>
         <stp>BDP|8619946037809089717</stp>
         <tr r="O73" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4046934780</v>
+        <v>#N/A Requesting Data...2801376890</v>
         <stp/>
         <stp>BDP|8134701725687838685</stp>
         <tr r="D101" s="2"/>
@@ -2528,13 +2532,13 @@
         <tr r="H141" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3677400983</v>
+        <v>#N/A Requesting Data...3439512723</v>
         <stp/>
         <stp>BDP|2337395976008307323</stp>
         <tr r="D133" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3105403371</v>
+        <v>#N/A Requesting Data...4149737066</v>
         <stp/>
         <stp>BDP|7346443724919908584</stp>
         <tr r="C143" s="2"/>
@@ -2548,55 +2552,55 @@
         <tr r="H47" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3781980446</v>
+        <v>#N/A Requesting Data...3555388658</v>
         <stp/>
         <stp>BDP|2452480886172944101</stp>
         <tr r="D83" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3038613679</v>
+        <v>#N/A Requesting Data...3977867653</v>
         <stp/>
         <stp>BDP|3988758046487897994</stp>
         <tr r="O100" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3004794482</v>
+        <v>#N/A Requesting Data...2591800360</v>
         <stp/>
         <stp>BDP|8487968754382467898</stp>
         <tr r="O111" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...889200744</v>
+        <v>#N/A Requesting Data...3027489072</v>
         <stp/>
         <stp>BDP|3168197062443776948</stp>
         <tr r="O97" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1660020218</v>
+        <v>#N/A Requesting Data...3684597067</v>
         <stp/>
         <stp>BDP|3191294011039253743</stp>
         <tr r="C100" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2981780643</v>
+        <v>#N/A Requesting Data...3849436575</v>
         <stp/>
         <stp>BDP|8158190943367710418</stp>
         <tr r="D141" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...770758056</v>
+        <v>#N/A Requesting Data...3201610832</v>
         <stp/>
         <stp>BDP|9753944506837726937</stp>
         <tr r="O139" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4173061278</v>
+        <v>#N/A Requesting Data...3709456892</v>
         <stp/>
         <stp>BDP|2383970352993755307</stp>
         <tr r="D111" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1515005215</v>
+        <v>#N/A Requesting Data...4173101373</v>
         <stp/>
         <stp>BDP|8422754563225257254</stp>
         <tr r="D119" s="2"/>
@@ -2610,67 +2614,67 @@
         <tr r="I103" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2123539436</v>
+        <v>#N/A Requesting Data...4067162888</v>
         <stp/>
         <stp>BDP|1905452132299753056</stp>
         <tr r="C39" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3128061408</v>
+        <v>#N/A Requesting Data...3908531200</v>
         <stp/>
         <stp>BDP|9168179234227771399</stp>
         <tr r="O128" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2597607997</v>
+        <v>#N/A Requesting Data...3740079716</v>
         <stp/>
         <stp>BDP|2740714101503839931</stp>
         <tr r="C141" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2384642291</v>
+        <v>#N/A Requesting Data...3378885159</v>
         <stp/>
         <stp>BDP|7992263003279543384</stp>
         <tr r="D142" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...630257197</v>
+        <v>#N/A Requesting Data...4060504464</v>
         <stp/>
         <stp>BDP|5477825144986453010</stp>
         <tr r="O59" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1903357743</v>
+        <v>#N/A Requesting Data...2661298930</v>
         <stp/>
         <stp>BDP|8165965388487479679</stp>
         <tr r="O81" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...780163365</v>
+        <v>#N/A Requesting Data...4000342018</v>
         <stp/>
         <stp>BDP|5675445137023195982</stp>
         <tr r="O143" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2651115773</v>
+        <v>#N/A Requesting Data...3547873559</v>
         <stp/>
         <stp>BDP|4173264548992531864</stp>
         <tr r="O109" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1754892212</v>
+        <v>#N/A Requesting Data...4080102033</v>
         <stp/>
         <stp>BDP|6322017615579378624</stp>
         <tr r="O90" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1724489614</v>
+        <v>#N/A Requesting Data...4014114839</v>
         <stp/>
         <stp>BDP|7700706960287514955</stp>
         <tr r="O99" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3025297419</v>
+        <v>#N/A Requesting Data...3025488650</v>
         <stp/>
         <stp>BDP|2684958064503521663</stp>
         <tr r="C87" s="2"/>
@@ -2684,7 +2688,7 @@
         <tr r="I143" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2070620030</v>
+        <v>#N/A Requesting Data...3417020872</v>
         <stp/>
         <stp>BDP|2825895505117461495</stp>
         <tr r="O57" s="2"/>
@@ -2698,13 +2702,13 @@
         <tr r="I141" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3030554880</v>
+        <v>#N/A Requesting Data...4264084157</v>
         <stp/>
         <stp>BDP|5555436835568594389</stp>
         <tr r="D145" s="2"/>
       </tp>
       <tp>
-        <v>80</v>
+        <v>120</v>
         <stp/>
         <stp>BDP|328381708441600475|22</stp>
         <stp>EEX3PMDE Index</stp>
@@ -2712,73 +2716,73 @@
         <tr r="I57" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1741741936</v>
+        <v>#N/A Requesting Data...4206267014</v>
         <stp/>
         <stp>BDP|4279202299077950281</stp>
         <tr r="D41" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2593765940</v>
+        <v>#N/A Requesting Data...2932312306</v>
         <stp/>
         <stp>BDP|6929810016462650737</stp>
         <tr r="D87" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3751561333</v>
+        <v>#N/A Requesting Data...3874833463</v>
         <stp/>
         <stp>BDP|1294936769142798640</stp>
         <tr r="C37" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1760122265</v>
+        <v>#N/A Requesting Data...2640453350</v>
         <stp/>
         <stp>BDP|8268735055277832754</stp>
         <tr r="D100" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1338630644</v>
+        <v>#N/A Requesting Data...2600774164</v>
         <stp/>
         <stp>BDP|7997415316799901193</stp>
         <tr r="O53" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2024293316</v>
+        <v>#N/A Requesting Data...4284854612</v>
         <stp/>
         <stp>BDP|6278897671657613432</stp>
         <tr r="O145" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1880982897</v>
+        <v>#N/A Requesting Data...2834725402</v>
         <stp/>
         <stp>BDP|8917206333941126276</stp>
         <tr r="O79" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3766734351</v>
+        <v>#N/A Requesting Data...3897705898</v>
         <stp/>
         <stp>BDP|9488941276259397490</stp>
         <tr r="O67" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1075630344</v>
+        <v>#N/A Requesting Data...3034077807</v>
         <stp/>
         <stp>BDP|5600386799382259784</stp>
         <tr r="C113" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...720912314</v>
+        <v>#N/A Requesting Data...2725841325</v>
         <stp/>
         <stp>BDP|9996435367631888077</stp>
         <tr r="C71" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1292773249</v>
+        <v>#N/A Requesting Data...3702604967</v>
         <stp/>
         <stp>BDP|3790921814431878090</stp>
         <tr r="D38" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3046430396</v>
+        <v>#N/A Requesting Data...3986815825</v>
         <stp/>
         <stp>BDP|5023633295787322705</stp>
         <tr r="C101" s="2"/>
@@ -2801,37 +2805,37 @@
         <tr r="H151" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2541017322</v>
+        <v>#N/A Requesting Data...4005354041</v>
         <stp/>
         <stp>BDP|2742897454442023636</stp>
         <tr r="D93" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1540514189</v>
+        <v>#N/A Requesting Data...3404185245</v>
         <stp/>
         <stp>BDP|1308380368217282806</stp>
         <tr r="C89" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4145025843</v>
+        <v>#N/A Requesting Data...3467202379</v>
         <stp/>
         <stp>BDP|2125519877263797874</stp>
         <tr r="D49" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1199127923</v>
+        <v>#N/A Requesting Data...3617669863</v>
         <stp/>
         <stp>BDP|8187334089870399738</stp>
         <tr r="C142" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1440353758</v>
+        <v>#N/A Requesting Data...3807226452</v>
         <stp/>
         <stp>BDP|8447705041427452887</stp>
         <tr r="O110" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1484393845</v>
+        <v>#N/A Requesting Data...4136202339</v>
         <stp/>
         <stp>BDP|9588220581862090554</stp>
         <tr r="D81" s="2"/>
@@ -2845,122 +2849,122 @@
         <tr r="H123" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3842863921</v>
+        <v>#N/A Requesting Data...3204592648</v>
         <stp/>
         <stp>BDP|6336981452218022714</stp>
         <tr r="D149" s="2"/>
         <tr r="D28" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3062714944</v>
+        <v>#N/A Requesting Data...4097339109</v>
         <stp/>
         <stp>BDP|5144982884240236131</stp>
         <tr r="O119" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4276137287</v>
+        <v>#N/A Requesting Data...3233638642</v>
         <stp/>
         <stp>BDP|4912389578430923538</stp>
         <tr r="C125" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2347478691</v>
+        <v>#N/A Requesting Data...3540704211</v>
         <stp/>
         <stp>BDP|4899183487030457834</stp>
         <tr r="D47" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1650866535</v>
+        <v>#N/A Requesting Data...3972335805</v>
         <stp/>
         <stp>BDP|7406447711566288126</stp>
         <tr r="O91" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3836089196</v>
+        <v>#N/A Requesting Data...3378496413</v>
         <stp/>
         <stp>BDP|2318106224533271732</stp>
         <tr r="D123" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1973466894</v>
+        <v>#N/A Requesting Data...2996942444</v>
         <stp/>
         <stp>BDP|5397604398148966497</stp>
         <tr r="C118" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2111870186</v>
+        <v>#N/A Requesting Data...2685948131</v>
         <stp/>
         <stp>BDP|5247213518087466774</stp>
         <tr r="D79" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3895303711</v>
+        <v>#N/A Requesting Data...3545188553</v>
         <stp/>
         <stp>BDP|2268502188811293879</stp>
         <tr r="O45" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1680162706</v>
+        <v>#N/A Requesting Data...3712260823</v>
         <stp/>
         <stp>BDP|2615106264042847162</stp>
         <tr r="C35" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3671360790</v>
+        <v>#N/A Requesting Data...3154800385</v>
         <stp/>
         <stp>BDP|7242668637610389424</stp>
         <tr r="C38" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3604749417</v>
+        <v>#N/A Requesting Data...2733665653</v>
         <stp/>
         <stp>BDP|3708410904060798168</stp>
         <tr r="D110" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2092639313</v>
+        <v>#N/A Requesting Data...3626484470</v>
         <stp/>
         <stp>BDP|5117711638166954114</stp>
         <tr r="O131" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2642314258</v>
+        <v>#N/A Requesting Data...4243454688</v>
         <stp/>
         <stp>BDP|3978038447362277279</stp>
         <tr r="O50" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2504881514</v>
+        <v>#N/A Requesting Data...4043975093</v>
         <stp/>
         <stp>BDP|4136828621258877131</stp>
         <tr r="C122" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2803971201</v>
+        <v>#N/A Requesting Data...3080849781</v>
         <stp/>
         <stp>BDP|2277297320794027172</stp>
         <tr r="O93" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3168409752</v>
+        <v>#N/A Requesting Data...4267652609</v>
         <stp/>
         <stp>BDP|8961196036758342506</stp>
         <tr r="D113" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2437484404</v>
+        <v>#N/A Requesting Data...3238207015</v>
         <stp/>
         <stp>BDP|1170165359530510519</stp>
         <tr r="C53" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1306253138</v>
+        <v>#N/A Requesting Data...3027240554</v>
         <stp/>
         <stp>BDP|3942355915051567002</stp>
         <tr r="C133" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3045320032</v>
+        <v>#N/A Requesting Data...3443694904</v>
         <stp/>
         <stp>BDP|3535326747745052123</stp>
         <tr r="D53" s="2"/>
@@ -2982,68 +2986,68 @@
         <tr r="H48" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3100514454</v>
+        <v>#N/A Requesting Data...2845089831</v>
         <stp/>
         <stp>BDP|9540225089557104556</stp>
         <tr r="O118" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2711076765</v>
+        <v>#N/A Requesting Data...2950042427</v>
         <stp/>
         <stp>BDP|5062514338582227013</stp>
         <tr r="D128" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3301257621</v>
+        <v>#N/A Requesting Data...3209131579</v>
         <stp/>
         <stp>BDP|2343600014653733789</stp>
         <tr r="O103" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2767610594</v>
+        <v>#N/A Requesting Data...3173845947</v>
         <stp/>
         <stp>BDP|3242086975802090723</stp>
         <tr r="D90" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1207243106</v>
+        <v>#N/A Requesting Data...2768187142</v>
         <stp/>
         <stp>BDP|8360886275346359094</stp>
         <tr r="C103" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1791019712</v>
+        <v>#N/A Requesting Data...2707859141</v>
         <stp/>
         <stp>BDP|6855110725440116773</stp>
         <tr r="C61" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2324761117</v>
+        <v>#N/A Requesting Data...3486981765</v>
         <stp/>
         <stp>BDP|8675841477756696315</stp>
         <tr r="C139" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1905174964</v>
+        <v>#N/A Requesting Data...3788455021</v>
         <stp/>
         <stp>BDP|4759583229459353843</stp>
         <tr r="O47" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3962987167</v>
+        <v>#N/A Requesting Data...3966089322</v>
         <stp/>
         <stp>BDP|9839782485004760030</stp>
         <tr r="C149" s="2"/>
         <tr r="C28" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2218783759</v>
+        <v>#N/A Requesting Data...3562887591</v>
         <stp/>
         <stp>BDP|3917864525078759387</stp>
         <tr r="C47" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...939049199</v>
+        <v>#N/A Requesting Data...3479945100</v>
         <stp/>
         <stp>BDP|1874573773983759306</stp>
         <tr r="C60" s="2"/>
@@ -3057,25 +3061,25 @@
         <tr r="H53" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4253445303</v>
+        <v>#N/A Requesting Data...3247486241</v>
         <stp/>
         <stp>BDP|4991441920223468278</stp>
         <tr r="C110" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1924948218</v>
+        <v>#N/A Requesting Data...2973918855</v>
         <stp/>
         <stp>BDP|4634330117701477447</stp>
         <tr r="D48" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2266782625</v>
+        <v>#N/A Requesting Data...3051520837</v>
         <stp/>
         <stp>BDP|3206597226223845400</stp>
         <tr r="D35" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4006369891</v>
+        <v>#N/A Requesting Data...3985688352</v>
         <stp/>
         <stp>BDP|7344440665766321042</stp>
         <tr r="D45" s="2"/>
@@ -3105,7 +3109,7 @@
         <tr r="I119" s="2"/>
       </tp>
       <tp>
-        <v>64</v>
+        <v>68</v>
         <stp/>
         <stp>BDP|5258715941910323221|22</stp>
         <stp>EEXXT3PA Index</stp>
@@ -3113,13 +3117,13 @@
         <tr r="H45" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...874446314</v>
+        <v>#N/A Requesting Data...2697543767</v>
         <stp/>
         <stp>BDP|92010296815936747</stp>
         <tr r="D132" s="2"/>
       </tp>
       <tp>
-        <v>85</v>
+        <v>80</v>
         <stp/>
         <stp>BDP|1716388539457443821|22</stp>
         <stp>EEXXT3PA Index</stp>
@@ -3199,7 +3203,7 @@
         <tr r="H129" s="2"/>
       </tp>
       <tp t="s">
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
         <stp/>
         <stp>BDP|3638041331352720978|22</stp>
         <stp>EEX33XPL Index</stp>
@@ -3207,7 +3211,7 @@
         <tr r="P89" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...722653750</v>
+        <v>#N/A Requesting Data...2918368134</v>
         <stp/>
         <stp>BDP|141486019989176878</stp>
         <tr r="C77" s="2"/>
@@ -3229,13 +3233,13 @@
         <tr r="I142" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...725845606</v>
+        <v>#N/A Requesting Data...3682123804</v>
         <stp/>
         <stp>BDP|498236031780937674</stp>
         <tr r="O71" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3940544965</v>
+        <v>#N/A Requesting Data...2872576755</v>
         <stp/>
         <stp>BDP|626474072446054250</stp>
         <tr r="O48" s="2"/>
@@ -3249,7 +3253,7 @@
         <tr r="I128" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...1819657025</v>
+        <v>#N/A Requesting Data...3788168275</v>
         <stp/>
         <stp>BDP|949597951093820562</stp>
         <tr r="C69" s="2"/>
@@ -3271,7 +3275,7 @@
         <tr r="I139" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2905691962</v>
+        <v>#N/A Requesting Data...3941630953</v>
         <stp/>
         <stp>BDP|527374345414391240</stp>
         <tr r="C99" s="2"/>
@@ -3285,13 +3289,13 @@
         <tr r="I38" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3521986730</v>
+        <v>#N/A Requesting Data...4067730845</v>
         <stp/>
         <stp>BDP|445371574551055651</stp>
         <tr r="C111" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Real Time</v>
+        <v>#N/A N/A</v>
         <stp/>
         <stp>BDP|17587492918187176311|22</stp>
         <stp>RGGIAAQS Index</stp>
@@ -3315,7 +3319,7 @@
         <tr r="H125" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3784117788</v>
+        <v>#N/A Requesting Data...3124867555</v>
         <stp/>
         <stp>BDP|411030222906237860</stp>
         <tr r="O133" s="2"/>
@@ -3385,7 +3389,7 @@
         <tr r="H39" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2206784597</v>
+        <v>#N/A Requesting Data...3226658399</v>
         <stp/>
         <stp>BDP|112394073414420858</stp>
         <tr r="C123" s="2"/>
@@ -3399,7 +3403,7 @@
         <tr r="I152" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3546987157</v>
+        <v>#N/A Requesting Data...3383355480</v>
         <stp/>
         <stp>BDP|280997264327962398</stp>
         <tr r="O149" s="2"/>
@@ -3471,7 +3475,7 @@
         <tr r="H49" s="2"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...2539283502</v>
+        <v>#N/A Requesting Data...3175611080</v>
         <stp/>
         <stp>BDP|599652034392309</stp>
         <tr r="D143" s="2"/>
@@ -3779,7 +3783,7 @@
   <dimension ref="A1:P152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:P24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4506,7 +4510,7 @@
       </c>
       <c r="C35">
         <f>_xll.BDP("UKAAUPR Index","PX_LAST")</f>
-        <v>49.95</v>
+        <v>53.55</v>
       </c>
       <c r="D35">
         <f>_xll.BDP("UKAAUPR Index","PX_VOLUME")</f>
@@ -4525,11 +4529,11 @@
       </c>
       <c r="O35" t="str">
         <f>_xll.BDP("UKAAUPR Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P35" t="str">
         <f>_xll.BDP("UKAAUPR Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -4549,7 +4553,7 @@
       </c>
       <c r="C37">
         <f>_xll.BDP("UKACORAT Index","PX_LAST")</f>
-        <v>1.5320527138708999</v>
+        <v>1.68215322760777</v>
       </c>
       <c r="D37" t="str">
         <f>_xll.BDP("UKACORAT Index","PX_VOLUME")</f>
@@ -4568,11 +4572,11 @@
       </c>
       <c r="O37" t="str">
         <f>_xll.BDP("UKACORAT Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P37" t="str">
         <f>_xll.BDP("UKACORAT Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -4584,7 +4588,7 @@
       </c>
       <c r="C38">
         <f>_xll.BDP("UKASBBID Index","PX_LAST")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D38">
         <f>_xll.BDP("UKASBBID Index","PX_VOLUME")</f>
@@ -4603,11 +4607,11 @@
       </c>
       <c r="O38" t="str">
         <f>_xll.BDP("UKASBBID Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P38" t="str">
         <f>_xll.BDP("UKASBBID Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -4619,7 +4623,7 @@
       </c>
       <c r="C39">
         <f>_xll.BDP("UKATOBID Index","PX_LAST")</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39">
         <f>_xll.BDP("UKATOBID Index","PX_VOLUME")</f>
@@ -4638,11 +4642,11 @@
       </c>
       <c r="O39" t="str">
         <f>_xll.BDP("UKATOBID Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P39" t="str">
         <f>_xll.BDP("UKATOBID Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -4662,7 +4666,7 @@
       </c>
       <c r="C41">
         <f>_xll.BDP("UKABIDS Index","PX_LAST")</f>
-        <v>3429500</v>
+        <v>3765500</v>
       </c>
       <c r="D41">
         <f>_xll.BDP("UKABIDS Index","PX_VOLUME")</f>
@@ -4681,11 +4685,11 @@
       </c>
       <c r="O41" t="str">
         <f>_xll.BDP("UKABIDS Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P41" t="str">
         <f>_xll.BDP("UKABIDS Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -4734,7 +4738,7 @@
       </c>
       <c r="C45">
         <f>_xll.BDP("EEXXT3PA Index","PX_LAST")</f>
-        <v>73.14</v>
+        <v>75.209999999999994</v>
       </c>
       <c r="D45">
         <f>_xll.BDP("EEXXT3PA Index","PX_VOLUME")</f>
@@ -4742,18 +4746,18 @@
       </c>
       <c r="H45">
         <f>_xll.BDP("EEXXT3PA Index","BID")</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I45">
         <f>_xll.BDP("EEXXT3PA Index","ASK")</f>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N45" t="s">
         <v>58</v>
       </c>
       <c r="O45" t="str">
         <f>_xll.BDP("EEXXT3PA Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P45" t="str">
         <f>_xll.BDP("EEXXT3PA Index","TIME")</f>
@@ -4777,7 +4781,7 @@
       </c>
       <c r="C47">
         <f>_xll.BDP("EEX3CRT3 Index","PX_LAST")</f>
-        <v>1.34</v>
+        <v>1.69</v>
       </c>
       <c r="D47">
         <f>_xll.BDP("EEX3CRT3 Index","PX_VOLUME")</f>
@@ -4796,7 +4800,7 @@
       </c>
       <c r="O47" t="str">
         <f>_xll.BDP("EEX3CRT3 Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P47" t="str">
         <f>_xll.BDP("EEX3CRT3 Index","TIME")</f>
@@ -4812,7 +4816,7 @@
       </c>
       <c r="C48">
         <f>_xll.BDP("EEX3MNT3 Index","PX_LAST")</f>
-        <v>73.239999999999995</v>
+        <v>75</v>
       </c>
       <c r="D48">
         <f>_xll.BDP("EEX3MNT3 Index","PX_VOLUME")</f>
@@ -4831,7 +4835,7 @@
       </c>
       <c r="O48" t="str">
         <f>_xll.BDP("EEX3MNT3 Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P48" t="str">
         <f>_xll.BDP("EEX3MNT3 Index","TIME")</f>
@@ -4847,7 +4851,7 @@
       </c>
       <c r="C49">
         <f>_xll.BDP("EEX3MDT3 Index","PX_LAST")</f>
-        <v>73.010000000000005</v>
+        <v>74.959999999999994</v>
       </c>
       <c r="D49">
         <f>_xll.BDP("EEX3MDT3 Index","PX_VOLUME")</f>
@@ -4866,7 +4870,7 @@
       </c>
       <c r="O49" t="str">
         <f>_xll.BDP("EEX3MDT3 Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P49" t="str">
         <f>_xll.BDP("EEX3MDT3 Index","TIME")</f>
@@ -4882,7 +4886,7 @@
       </c>
       <c r="C50">
         <f>_xll.BDP("EEX3SCCB Index","PX_LAST")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D50">
         <f>_xll.BDP("EEX3SCCB Index","PX_VOLUME")</f>
@@ -4901,7 +4905,7 @@
       </c>
       <c r="O50" t="str">
         <f>_xll.BDP("EEX3SCCB Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P50" t="str">
         <f>_xll.BDP("EEX3SCCB Index","TIME")</f>
@@ -4936,7 +4940,7 @@
       </c>
       <c r="O51" t="str">
         <f>_xll.BDP("EEX3TOTB Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P51" t="str">
         <f>_xll.BDP("EEX3TOTB Index","TIME")</f>
@@ -4963,7 +4967,7 @@
       </c>
       <c r="C53">
         <f>_xll.BDP("EEX3BDT3 Index","PX_LAST")</f>
-        <v>4365500</v>
+        <v>5514500</v>
       </c>
       <c r="D53">
         <f>_xll.BDP("EEX3BDT3 Index","PX_VOLUME")</f>
@@ -4982,7 +4986,7 @@
       </c>
       <c r="O53" t="str">
         <f>_xll.BDP("EEX3BDT3 Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P53" t="str">
         <f>_xll.BDP("EEX3BDT3 Index","TIME")</f>
@@ -5035,30 +5039,30 @@
       </c>
       <c r="C57">
         <f>_xll.BDP("EEX3PMDE Index","PX_LAST")</f>
-        <v>71.3</v>
+        <v>75.44</v>
       </c>
       <c r="D57">
         <f>_xll.BDP("EEX3PMDE Index","PX_VOLUME")</f>
-        <v>1614500</v>
+        <v>1691000</v>
       </c>
       <c r="H57">
         <f>_xll.BDP("EEX3PMDE Index","BID")</f>
-        <v>65</v>
+        <v>73.2</v>
       </c>
       <c r="I57">
         <f>_xll.BDP("EEX3PMDE Index","ASK")</f>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="N57" t="s">
         <v>61</v>
       </c>
       <c r="O57" t="str">
         <f>_xll.BDP("EEX3PMDE Index","LAST_UPDATE_DT")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
       <c r="P57" t="str">
         <f>_xll.BDP("EEX3PMDE Index","TIME")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -5078,7 +5082,7 @@
       </c>
       <c r="C59">
         <f>_xll.BDP("EEX3CRDE Index","PX_LAST")</f>
-        <v>1.82</v>
+        <v>1.75</v>
       </c>
       <c r="D59">
         <f>_xll.BDP("EEX3CRDE Index","PX_VOLUME")</f>
@@ -5097,11 +5101,11 @@
       </c>
       <c r="O59" t="str">
         <f>_xll.BDP("EEX3CRDE Index","LAST_UPDATE_DT")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
       <c r="P59" t="str">
         <f>_xll.BDP("EEX3CRDE Index","TIME")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -5113,7 +5117,7 @@
       </c>
       <c r="C60">
         <f>_xll.BDP("EEX3MNDE Index","PX_LAST")</f>
-        <v>71.73</v>
+        <v>75.97</v>
       </c>
       <c r="D60">
         <f>_xll.BDP("EEX3MNDE Index","PX_VOLUME")</f>
@@ -5132,11 +5136,11 @@
       </c>
       <c r="O60" t="str">
         <f>_xll.BDP("EEX3MNDE Index","LAST_UPDATE_DT")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
       <c r="P60" t="str">
         <f>_xll.BDP("EEX3MNDE Index","TIME")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -5148,7 +5152,7 @@
       </c>
       <c r="C61">
         <f>_xll.BDP("EEX3MDDE Index","PX_LAST")</f>
-        <v>71.17</v>
+        <v>75.31</v>
       </c>
       <c r="D61">
         <f>_xll.BDP("EEX3MDDE Index","PX_VOLUME")</f>
@@ -5167,11 +5171,11 @@
       </c>
       <c r="O61" t="str">
         <f>_xll.BDP("EEX3MDDE Index","LAST_UPDATE_DT")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
       <c r="P61" t="str">
         <f>_xll.BDP("EEX3MDDE Index","TIME")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -5194,7 +5198,7 @@
       </c>
       <c r="C63">
         <f>_xll.BDP("EEX3BDDE Index","PX_LAST")</f>
-        <v>2932500</v>
+        <v>2964000</v>
       </c>
       <c r="D63">
         <f>_xll.BDP("EEX3BDDE Index","PX_VOLUME")</f>
@@ -5213,11 +5217,11 @@
       </c>
       <c r="O63" t="str">
         <f>_xll.BDP("EEX3BDDE Index","LAST_UPDATE_DT")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
       <c r="P63" t="str">
         <f>_xll.BDP("EEX3BDDE Index","TIME")</f>
-        <v>29.08.2025</v>
+        <v>05.09.2025</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -5266,7 +5270,7 @@
       </c>
       <c r="C67">
         <f>_xll.BDP("EEX3EPPM Index","PX_LAST")</f>
-        <v>73.14</v>
+        <v>75.209999999999994</v>
       </c>
       <c r="D67">
         <f>_xll.BDP("EEX3EPPM Index","PX_VOLUME")</f>
@@ -5274,22 +5278,22 @@
       </c>
       <c r="H67">
         <f>_xll.BDP("EEX3EPPM Index","BID")</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I67">
         <f>_xll.BDP("EEX3EPPM Index","ASK")</f>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N67" t="s">
         <v>63</v>
       </c>
       <c r="O67" t="str">
         <f>_xll.BDP("EEX3EPPM Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P67" t="str">
         <f>_xll.BDP("EEX3EPPM Index","TIME")</f>
-        <v>11:00:32</v>
+        <v>11:00:34</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -5309,7 +5313,7 @@
       </c>
       <c r="C69">
         <f>_xll.BDP("EEX3EPCR Index","PX_LAST")</f>
-        <v>1.34</v>
+        <v>1.69</v>
       </c>
       <c r="D69">
         <f>_xll.BDP("EEX3EPCR Index","PX_VOLUME")</f>
@@ -5328,7 +5332,7 @@
       </c>
       <c r="O69" t="str">
         <f>_xll.BDP("EEX3EPCR Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P69" t="str">
         <f>_xll.BDP("EEX3EPCR Index","TIME")</f>
@@ -5344,7 +5348,7 @@
       </c>
       <c r="C70">
         <f>_xll.BDP("EEX3MNEP Index","PX_LAST")</f>
-        <v>73.239999999999995</v>
+        <v>75</v>
       </c>
       <c r="D70">
         <f>_xll.BDP("EEX3MNEP Index","PX_VOLUME")</f>
@@ -5363,7 +5367,7 @@
       </c>
       <c r="O70" t="str">
         <f>_xll.BDP("EEX3MNEP Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P70" t="str">
         <f>_xll.BDP("EEX3MNEP Index","TIME")</f>
@@ -5379,7 +5383,7 @@
       </c>
       <c r="C71">
         <f>_xll.BDP("EEX3MDEP Index","PX_LAST")</f>
-        <v>73.010000000000005</v>
+        <v>74.959999999999994</v>
       </c>
       <c r="D71">
         <f>_xll.BDP("EEX3MDEP Index","PX_VOLUME")</f>
@@ -5398,7 +5402,7 @@
       </c>
       <c r="O71" t="str">
         <f>_xll.BDP("EEX3MDEP Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P71" t="str">
         <f>_xll.BDP("EEX3MDEP Index","TIME")</f>
@@ -5425,7 +5429,7 @@
       </c>
       <c r="C73">
         <f>_xll.BDP("EEX3BDEP Index","PX_LAST")</f>
-        <v>4365500</v>
+        <v>5514500</v>
       </c>
       <c r="D73">
         <f>_xll.BDP("EEX3BDEP Index","PX_VOLUME")</f>
@@ -5444,7 +5448,7 @@
       </c>
       <c r="O73" t="str">
         <f>_xll.BDP("EEX3BDEP Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P73" t="str">
         <f>_xll.BDP("EEX3BDEP Index","TIME")</f>
@@ -5497,7 +5501,7 @@
       </c>
       <c r="C77">
         <f>_xll.BDP("EEX3PMEU Index","PX_LAST")</f>
-        <v>73.14</v>
+        <v>75.209999999999994</v>
       </c>
       <c r="D77">
         <f>_xll.BDP("EEX3PMEU Index","PX_VOLUME")</f>
@@ -5505,18 +5509,18 @@
       </c>
       <c r="H77">
         <f>_xll.BDP("EEX3PMEU Index","BID")</f>
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I77">
         <f>_xll.BDP("EEX3PMEU Index","ASK")</f>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N77" t="s">
         <v>65</v>
       </c>
       <c r="O77" t="str">
         <f>_xll.BDP("EEX3PMEU Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P77" t="str">
         <f>_xll.BDP("EEX3PMEU Index","TIME")</f>
@@ -5540,7 +5544,7 @@
       </c>
       <c r="C79">
         <f>_xll.BDP("EEX3CREU Index","PX_LAST")</f>
-        <v>1.34</v>
+        <v>1.69</v>
       </c>
       <c r="D79">
         <f>_xll.BDP("EEX3CREU Index","PX_VOLUME")</f>
@@ -5559,7 +5563,7 @@
       </c>
       <c r="O79" t="str">
         <f>_xll.BDP("EEX3CREU Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P79" t="str">
         <f>_xll.BDP("EEX3CREU Index","TIME")</f>
@@ -5575,7 +5579,7 @@
       </c>
       <c r="C80">
         <f>_xll.BDP("EEX3MNEU Index","PX_LAST")</f>
-        <v>73.239999999999995</v>
+        <v>75</v>
       </c>
       <c r="D80">
         <f>_xll.BDP("EEX3MNEU Index","PX_VOLUME")</f>
@@ -5594,7 +5598,7 @@
       </c>
       <c r="O80" t="str">
         <f>_xll.BDP("EEX3MNEU Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P80" t="str">
         <f>_xll.BDP("EEX3MNEU Index","TIME")</f>
@@ -5610,7 +5614,7 @@
       </c>
       <c r="C81">
         <f>_xll.BDP("EEX3MDEU Index","PX_LAST")</f>
-        <v>73.010000000000005</v>
+        <v>74.959999999999994</v>
       </c>
       <c r="D81">
         <f>_xll.BDP("EEX3MDEU Index","PX_VOLUME")</f>
@@ -5629,7 +5633,7 @@
       </c>
       <c r="O81" t="str">
         <f>_xll.BDP("EEX3MDEU Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P81" t="str">
         <f>_xll.BDP("EEX3MDEU Index","TIME")</f>
@@ -5656,7 +5660,7 @@
       </c>
       <c r="C83">
         <f>_xll.BDP("EEX3BDEU Index","PX_LAST")</f>
-        <v>4365500</v>
+        <v>5514500</v>
       </c>
       <c r="D83">
         <f>_xll.BDP("EEX3BDEU Index","PX_VOLUME")</f>
@@ -5675,7 +5679,7 @@
       </c>
       <c r="O83" t="str">
         <f>_xll.BDP("EEX3BDEU Index","LAST_UPDATE_DT")</f>
-        <v>01.09.2025</v>
+        <v>08.09.2025</v>
       </c>
       <c r="P83" t="str">
         <f>_xll.BDP("EEX3BDEU Index","TIME")</f>
@@ -5728,15 +5732,15 @@
       </c>
       <c r="C87">
         <f>_xll.BDP("EEX3X3PL Index","PX_LAST")</f>
-        <v>70.47</v>
+        <v>73.27</v>
       </c>
       <c r="D87">
         <f>_xll.BDP("EEX3X3PL Index","PX_VOLUME")</f>
-        <v>2069000</v>
+        <v>2162500</v>
       </c>
       <c r="H87">
         <f>_xll.BDP("EEX3X3PL Index","BID")</f>
-        <v>68.05</v>
+        <v>64</v>
       </c>
       <c r="I87">
         <f>_xll.BDP("EEX3X3PL Index","ASK")</f>
@@ -5747,11 +5751,11 @@
       </c>
       <c r="O87" t="str">
         <f>_xll.BDP("EEX3X3PL Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P87" t="str">
         <f>_xll.BDP("EEX3X3PL Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -5771,7 +5775,7 @@
       </c>
       <c r="C89">
         <f>_xll.BDP("EEX33XPL Index","PX_LAST")</f>
-        <v>1.66</v>
+        <v>1.44</v>
       </c>
       <c r="D89">
         <f>_xll.BDP("EEX33XPL Index","PX_VOLUME")</f>
@@ -5790,11 +5794,11 @@
       </c>
       <c r="O89" t="str">
         <f>_xll.BDP("EEX33XPL Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P89" t="str">
         <f>_xll.BDP("EEX33XPL Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -5806,7 +5810,7 @@
       </c>
       <c r="C90">
         <f>_xll.BDP("EEX3MNPL Index","PX_LAST")</f>
-        <v>70.540000000000006</v>
+        <v>73.239999999999995</v>
       </c>
       <c r="D90">
         <f>_xll.BDP("EEX3MNPL Index","PX_VOLUME")</f>
@@ -5825,11 +5829,11 @@
       </c>
       <c r="O90" t="str">
         <f>_xll.BDP("EEX3MNPL Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P90" t="str">
         <f>_xll.BDP("EEX3MNPL Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -5841,7 +5845,7 @@
       </c>
       <c r="C91">
         <f>_xll.BDP("EEX3MDPL Index","PX_LAST")</f>
-        <v>70.150000000000006</v>
+        <v>73.17</v>
       </c>
       <c r="D91">
         <f>_xll.BDP("EEX3MDPL Index","PX_VOLUME")</f>
@@ -5860,11 +5864,11 @@
       </c>
       <c r="O91" t="str">
         <f>_xll.BDP("EEX3MDPL Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P91" t="str">
         <f>_xll.BDP("EEX3MDPL Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -5887,7 +5891,7 @@
       </c>
       <c r="C93">
         <f>_xll.BDP("EEX3BDPL Index","PX_LAST")</f>
-        <v>3428000</v>
+        <v>3118500</v>
       </c>
       <c r="D93">
         <f>_xll.BDP("EEX3BDPL Index","PX_VOLUME")</f>
@@ -5906,11 +5910,11 @@
       </c>
       <c r="O93" t="str">
         <f>_xll.BDP("EEX3BDPL Index","LAST_UPDATE_DT")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P93" t="str">
         <f>_xll.BDP("EEX3BDPL Index","TIME")</f>
-        <v>20.08.2025</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -6995,7 +6999,7 @@
       </c>
       <c r="C141">
         <f>_xll.BDP("RGGIAROB Index","PX_LAST")</f>
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="D141" t="str">
         <f>_xll.BDP("RGGIAROB Index","PX_VOLUME")</f>
@@ -7014,7 +7018,7 @@
       </c>
       <c r="O141" t="str">
         <f>_xll.BDP("RGGIAROB Index","LAST_UPDATE_DT")</f>
-        <v>04.06.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P141" t="str">
         <f>_xll.BDP("RGGIAROB Index","TIME")</f>
@@ -7108,7 +7112,7 @@
       </c>
       <c r="C145">
         <f>_xll.BDP("RGGIAAQS Index","PX_LAST")</f>
-        <v>15244480</v>
+        <v>15177780</v>
       </c>
       <c r="D145" t="str">
         <f>_xll.BDP("RGGIAAQS Index","PX_VOLUME")</f>
@@ -7116,22 +7120,22 @@
       </c>
       <c r="H145" t="str">
         <f>_xll.BDP("RGGIAAQS Index","BID")</f>
-        <v>#N/A Real Time</v>
+        <v>#N/A N/A</v>
       </c>
       <c r="I145" t="str">
         <f>_xll.BDP("RGGIAAQS Index","ASK")</f>
-        <v>#N/A Real Time</v>
+        <v>#N/A N/A</v>
       </c>
       <c r="N145" t="s">
         <v>80</v>
       </c>
       <c r="O145" t="str">
         <f>_xll.BDP("RGGIAAQS Index","LAST_UPDATE_DT")</f>
-        <v>04.06.2025</v>
+        <v>03.09.2025</v>
       </c>
       <c r="P145" t="str">
         <f>_xll.BDP("RGGIAAQS Index","TIME")</f>
-        <v>#N/A Real Time</v>
+        <v>03.09.2025</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
@@ -7262,26 +7266,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A115:P115"/>
+    <mergeCell ref="A116:P116"/>
+    <mergeCell ref="A126:P126"/>
+    <mergeCell ref="A137:P137"/>
+    <mergeCell ref="A147:P147"/>
+    <mergeCell ref="A65:P65"/>
+    <mergeCell ref="A75:P75"/>
+    <mergeCell ref="A85:P85"/>
+    <mergeCell ref="A95:P95"/>
+    <mergeCell ref="A105:P105"/>
+    <mergeCell ref="A30:P30"/>
+    <mergeCell ref="A31:P31"/>
+    <mergeCell ref="A33:P33"/>
+    <mergeCell ref="A43:P43"/>
+    <mergeCell ref="A55:P55"/>
     <mergeCell ref="A2:P2"/>
     <mergeCell ref="A5:P5"/>
     <mergeCell ref="A19:P19"/>
     <mergeCell ref="A24:P24"/>
     <mergeCell ref="A27:P27"/>
-    <mergeCell ref="A30:P30"/>
-    <mergeCell ref="A31:P31"/>
-    <mergeCell ref="A33:P33"/>
-    <mergeCell ref="A43:P43"/>
-    <mergeCell ref="A55:P55"/>
-    <mergeCell ref="A65:P65"/>
-    <mergeCell ref="A75:P75"/>
-    <mergeCell ref="A85:P85"/>
-    <mergeCell ref="A95:P95"/>
-    <mergeCell ref="A105:P105"/>
-    <mergeCell ref="A115:P115"/>
-    <mergeCell ref="A116:P116"/>
-    <mergeCell ref="A126:P126"/>
-    <mergeCell ref="A137:P137"/>
-    <mergeCell ref="A147:P147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>